<commit_message>
made changes to excel file
</commit_message>
<xml_diff>
--- a/Schedule_aw.xlsx
+++ b/Schedule_aw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Fulltime/Part-time</t>
   </si>
   <si>
+    <t>Tier</t>
+  </si>
+  <si>
     <t>Arun</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
     <t>Fulltime</t>
   </si>
   <si>
+    <t>Tier 1</t>
+  </si>
+  <si>
     <t>Christo</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
     <t>Part-time</t>
   </si>
   <si>
+    <t>Tier 2</t>
+  </si>
+  <si>
     <t>Rishitha</t>
   </si>
   <si>
@@ -93,6 +102,9 @@
   </si>
   <si>
     <t>Tue,Wed</t>
+  </si>
+  <si>
+    <t>Tier 3</t>
   </si>
   <si>
     <t>Person11</t>
@@ -1297,13 +1309,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D23"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="23.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="24.2857142857143" customWidth="1"/>
@@ -1311,7 +1323,7 @@
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1324,313 +1336,382 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>